<commit_message>
JS + html flow from MADtrial
</commit_message>
<xml_diff>
--- a/app/config/tables/Limpeza/Forms/Limpeza/Limpeza.xlsx
+++ b/app/config/tables/Limpeza/Forms/Limpeza/Limpeza.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001286BB-F2D2-448B-A73F-5FB3006A8287}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5F26AA-08C0-43B8-A155-FAAC3370F42E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>setting_name</t>
   </si>
@@ -176,7 +176,25 @@
     <t>App de Limpeza de Dadaos de Bandim (Exemplo)</t>
   </si>
   <si>
-    <t>This is an example</t>
+    <t>Info screen</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>data("ERROR1") == "1"</t>
+  </si>
+  <si>
+    <t>end if</t>
+  </si>
+  <si>
+    <t>data("ERROR2") == "2"</t>
+  </si>
+  <si>
+    <t>Cleaning of error 1</t>
+  </si>
+  <si>
+    <t>Cleaning of error 2</t>
   </si>
 </sst>
 </file>
@@ -684,12 +702,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787AB6FC-E5B2-448F-8A60-6571052C1548}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,6 +789,74 @@
         <v>40</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -783,7 +869,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D16"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>